<commit_message>
copy (not move) loc data from tourney sheets. in prep for code change.
</commit_message>
<xml_diff>
--- a/src/stp/database/2018-mens-world-cup.xlsx
+++ b/src/stp/database/2018-mens-world-cup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/src/stp/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37A55AE0-29E6-C747-AB4A-73EA1A14619B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90B9CFF-DECF-3A49-BA1C-081F239411D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19280" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="38400" windowHeight="19280" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tournament" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="214">
   <si>
     <t>A1</t>
   </si>
@@ -597,6 +597,90 @@
   </si>
   <si>
     <t>جام جهانی</t>
+  </si>
+  <si>
+    <t>venue-key.1</t>
+  </si>
+  <si>
+    <t>ru-moscow_luzhniki</t>
+  </si>
+  <si>
+    <t>venue-key.2</t>
+  </si>
+  <si>
+    <t>ru-ekaterinburg</t>
+  </si>
+  <si>
+    <t>venue-key.3</t>
+  </si>
+  <si>
+    <t>ru-saint-petersburg</t>
+  </si>
+  <si>
+    <t>venue-key.4</t>
+  </si>
+  <si>
+    <t>ru-sochi</t>
+  </si>
+  <si>
+    <t>venue-key.5</t>
+  </si>
+  <si>
+    <t>ru-kazan</t>
+  </si>
+  <si>
+    <t>venue-key.6</t>
+  </si>
+  <si>
+    <t>ru-moscow_otkrytiye</t>
+  </si>
+  <si>
+    <t>venue-key.7</t>
+  </si>
+  <si>
+    <t>ru-saransk</t>
+  </si>
+  <si>
+    <t>venue-key.8</t>
+  </si>
+  <si>
+    <t>ru-kaliningrad</t>
+  </si>
+  <si>
+    <t>venue-key.9</t>
+  </si>
+  <si>
+    <t>ru-samara</t>
+  </si>
+  <si>
+    <t>venue-key.10</t>
+  </si>
+  <si>
+    <t>ru-rostov-on-don</t>
+  </si>
+  <si>
+    <t>venue-key.11</t>
+  </si>
+  <si>
+    <t>ru-nizhny-novgorod</t>
+  </si>
+  <si>
+    <t>venue-key.12</t>
+  </si>
+  <si>
+    <t>ru-volgograd</t>
+  </si>
+  <si>
+    <t>competition-key</t>
+  </si>
+  <si>
+    <t>mens-world-cup</t>
+  </si>
+  <si>
+    <t>host-key</t>
+  </si>
+  <si>
+    <t>russia</t>
   </si>
 </sst>
 </file>
@@ -691,8 +775,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A35F1197-A800-47A7-9FB8-27BA1E42FC3F}" name="tournament" displayName="tournament" ref="A1:I16" totalsRowShown="0">
-  <autoFilter ref="A1:I16" xr:uid="{A35F1197-A800-47A7-9FB8-27BA1E42FC3F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A35F1197-A800-47A7-9FB8-27BA1E42FC3F}" name="tournament" displayName="tournament" ref="A1:I30" totalsRowShown="0">
+  <autoFilter ref="A1:I30" xr:uid="{A35F1197-A800-47A7-9FB8-27BA1E42FC3F}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A8CDEDD3-FA49-4AD4-8D9F-D3DFCABC2052}" name="key"/>
     <tableColumn id="2" xr3:uid="{88778009-1F1A-4B0F-BCE2-A71F4DD7CF67}" name="en"/>
@@ -1055,13 +1139,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393FFACE-29F0-47F7-B7AD-389E0D6667C5}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:I2"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1108,164 +1192,276 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>210</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G2" t="s">
-        <v>183</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="I2" t="s">
-        <v>185</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>212</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F3" t="s">
-        <v>174</v>
-      </c>
-      <c r="G3" t="s">
-        <v>175</v>
-      </c>
-      <c r="H3" t="s">
-        <v>176</v>
-      </c>
-      <c r="I3" t="s">
-        <v>177</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>170</v>
+        <v>114</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>178</v>
+      </c>
+      <c r="C4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" t="s">
+        <v>180</v>
+      </c>
+      <c r="E4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F4" t="s">
+        <v>182</v>
+      </c>
+      <c r="G4" t="s">
+        <v>183</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I4" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>124</v>
+      </c>
+      <c r="C5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E5" t="s">
+        <v>173</v>
+      </c>
+      <c r="F5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H5" t="s">
+        <v>176</v>
+      </c>
+      <c r="I5" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>101</v>
+        <v>170</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>171</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B7" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="B13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="B14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B17" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>128</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>186</v>
+      </c>
+      <c r="B19" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>188</v>
+      </c>
+      <c r="B20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>192</v>
+      </c>
+      <c r="B22" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>194</v>
+      </c>
+      <c r="B23" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>198</v>
+      </c>
+      <c r="B25" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>200</v>
+      </c>
+      <c r="B26" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>202</v>
+      </c>
+      <c r="B27" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>204</v>
+      </c>
+      <c r="B28" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>206</v>
+      </c>
+      <c r="B29" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>208</v>
+      </c>
+      <c r="B30" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
properties to properties tabs of tourney sheets
</commit_message>
<xml_diff>
--- a/src/stp/database/2018-mens-world-cup.xlsx
+++ b/src/stp/database/2018-mens-world-cup.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/src/stp/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90B9CFF-DECF-3A49-BA1C-081F239411D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB5F5D5-86DF-534F-B543-D0BDF358132F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="38400" windowHeight="19280" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19280" activeTab="4" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Tournament" sheetId="8" r:id="rId1"/>
     <sheet name="Matches" sheetId="1" r:id="rId2"/>
     <sheet name="Seeds" sheetId="3" r:id="rId3"/>
     <sheet name="Colors" sheetId="9" r:id="rId4"/>
+    <sheet name="Properties" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="228">
   <si>
     <t>A1</t>
   </si>
@@ -599,88 +600,130 @@
     <t>جام جهانی</t>
   </si>
   <si>
-    <t>venue-key.1</t>
-  </si>
-  <si>
     <t>ru-moscow_luzhniki</t>
   </si>
   <si>
-    <t>venue-key.2</t>
-  </si>
-  <si>
     <t>ru-ekaterinburg</t>
   </si>
   <si>
-    <t>venue-key.3</t>
-  </si>
-  <si>
     <t>ru-saint-petersburg</t>
   </si>
   <si>
-    <t>venue-key.4</t>
-  </si>
-  <si>
     <t>ru-sochi</t>
   </si>
   <si>
-    <t>venue-key.5</t>
-  </si>
-  <si>
     <t>ru-kazan</t>
   </si>
   <si>
-    <t>venue-key.6</t>
-  </si>
-  <si>
     <t>ru-moscow_otkrytiye</t>
   </si>
   <si>
-    <t>venue-key.7</t>
-  </si>
-  <si>
     <t>ru-saransk</t>
   </si>
   <si>
-    <t>venue-key.8</t>
-  </si>
-  <si>
     <t>ru-kaliningrad</t>
   </si>
   <si>
-    <t>venue-key.9</t>
-  </si>
-  <si>
     <t>ru-samara</t>
   </si>
   <si>
-    <t>venue-key.10</t>
-  </si>
-  <si>
     <t>ru-rostov-on-don</t>
   </si>
   <si>
-    <t>venue-key.11</t>
-  </si>
-  <si>
     <t>ru-nizhny-novgorod</t>
   </si>
   <si>
-    <t>venue-key.12</t>
-  </si>
-  <si>
     <t>ru-volgograd</t>
   </si>
   <si>
-    <t>competition-key</t>
-  </si>
-  <si>
     <t>mens-world-cup</t>
   </si>
   <si>
-    <t>host-key</t>
-  </si>
-  <si>
     <t>russia</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>color.a</t>
+  </si>
+  <si>
+    <t>color.b</t>
+  </si>
+  <si>
+    <t>color.c</t>
+  </si>
+  <si>
+    <t>color.d</t>
+  </si>
+  <si>
+    <t>color.e</t>
+  </si>
+  <si>
+    <t>color.f</t>
+  </si>
+  <si>
+    <t>color.g</t>
+  </si>
+  <si>
+    <t>color.h</t>
+  </si>
+  <si>
+    <t>venue.01</t>
+  </si>
+  <si>
+    <t>venue.02</t>
+  </si>
+  <si>
+    <t>venue.03</t>
+  </si>
+  <si>
+    <t>venue.04</t>
+  </si>
+  <si>
+    <t>venue.05</t>
+  </si>
+  <si>
+    <t>venue.06</t>
+  </si>
+  <si>
+    <t>venue.07</t>
+  </si>
+  <si>
+    <t>venue.08</t>
+  </si>
+  <si>
+    <t>venue.09</t>
+  </si>
+  <si>
+    <t>competition</t>
+  </si>
+  <si>
+    <t>host</t>
+  </si>
+  <si>
+    <t>cyan</t>
+  </si>
+  <si>
+    <t>yellow</t>
+  </si>
+  <si>
+    <t>red</t>
+  </si>
+  <si>
+    <t>green</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>teal</t>
+  </si>
+  <si>
+    <t>orange</t>
+  </si>
+  <si>
+    <t>purple</t>
   </si>
 </sst>
 </file>
@@ -736,7 +779,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -775,8 +821,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A35F1197-A800-47A7-9FB8-27BA1E42FC3F}" name="tournament" displayName="tournament" ref="A1:I30" totalsRowShown="0">
-  <autoFilter ref="A1:I30" xr:uid="{A35F1197-A800-47A7-9FB8-27BA1E42FC3F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A35F1197-A800-47A7-9FB8-27BA1E42FC3F}" name="tournament" displayName="tournament" ref="A1:I16" totalsRowShown="0">
+  <autoFilter ref="A1:I16" xr:uid="{A35F1197-A800-47A7-9FB8-27BA1E42FC3F}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A8CDEDD3-FA49-4AD4-8D9F-D3DFCABC2052}" name="key"/>
     <tableColumn id="2" xr3:uid="{88778009-1F1A-4B0F-BCE2-A71F4DD7CF67}" name="en"/>
@@ -799,14 +845,14 @@
     <tableColumn id="1" xr3:uid="{35D3E9F5-BB3B-4940-9EB6-C927FD84875C}" name="match"/>
     <tableColumn id="2" xr3:uid="{97337EE3-AAC3-4452-8381-1A56C6B35138}" name="home-seed"/>
     <tableColumn id="3" xr3:uid="{AEDB8750-5B25-4357-9054-E49FECC94717}" name="away-seed"/>
-    <tableColumn id="4" xr3:uid="{B178F43D-E631-4314-9E59-2CDA6EDA94F1}" name="time" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{398EE86D-DB71-4B07-BCF3-5E13F225DA53}" name="venue" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{68E01095-6C68-42AF-8716-32FC9C3B5D8B}" name="home-team" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{2CDCD506-6640-41AE-846E-162E81849C6B}" name="away-team" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{B178F43D-E631-4314-9E59-2CDA6EDA94F1}" name="time" dataDxfId="8"/>
+    <tableColumn id="16" xr3:uid="{398EE86D-DB71-4B07-BCF3-5E13F225DA53}" name="venue" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{68E01095-6C68-42AF-8716-32FC9C3B5D8B}" name="home-team" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{2CDCD506-6640-41AE-846E-162E81849C6B}" name="away-team" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -835,8 +881,23 @@
     <tableColumn id="6" xr3:uid="{1D61E46B-3B2C-4922-9B65-C97BF9F3EF2D}" name="de"/>
     <tableColumn id="7" xr3:uid="{6243B05C-6BAE-4D3D-9B50-8E8C73F0BCD4}" name="nl"/>
     <tableColumn id="8" xr3:uid="{6119E755-9CCC-4ABE-99D9-63CBF4D891CB}" name="ja"/>
-    <tableColumn id="9" xr3:uid="{12D54549-EC84-4A42-ACAB-B413320B4F44}" name="fa"/>
+    <tableColumn id="9" xr3:uid="{12D54549-EC84-4A42-ACAB-B413320B4F44}" name="fa" dataDxfId="0"/>
     <tableColumn id="10" xr3:uid="{1AF993A1-3EBC-4103-B829-4C6FDE197432}" name="notes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AEEE4923-055B-A14A-9B48-3E0283A1160B}" name="Properties" displayName="Properties" ref="A1:C24" totalsRowShown="0">
+  <autoFilter ref="A1:C24" xr:uid="{AEEE4923-055B-A14A-9B48-3E0283A1160B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C24">
+    <sortCondition ref="A1:A24"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{31E242A4-4364-304E-A4A7-4443C29CFCC1}" name="key"/>
+    <tableColumn id="2" xr3:uid="{7AFBD417-707A-F242-BB43-CEC5BB264EDA}" name="value"/>
+    <tableColumn id="3" xr3:uid="{4306B17E-8C36-1A4B-BF13-4EB899EF33B6}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1139,13 +1200,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393FFACE-29F0-47F7-B7AD-389E0D6667C5}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:XFD3"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17:XFD28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1192,276 +1253,164 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>210</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>211</v>
+        <v>178</v>
+      </c>
+      <c r="C2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" t="s">
+        <v>182</v>
+      </c>
+      <c r="G2" t="s">
+        <v>183</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="I2" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>212</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>213</v>
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G3" t="s">
+        <v>175</v>
+      </c>
+      <c r="H3" t="s">
+        <v>176</v>
+      </c>
+      <c r="I3" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>170</v>
       </c>
       <c r="B4" t="s">
-        <v>178</v>
-      </c>
-      <c r="C4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D4" t="s">
-        <v>180</v>
-      </c>
-      <c r="E4" t="s">
-        <v>181</v>
-      </c>
-      <c r="F4" t="s">
-        <v>182</v>
-      </c>
-      <c r="G4" t="s">
-        <v>183</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="I4" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
-      </c>
-      <c r="C5" t="s">
-        <v>172</v>
-      </c>
-      <c r="D5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E5" t="s">
-        <v>173</v>
-      </c>
-      <c r="F5" t="s">
-        <v>174</v>
-      </c>
-      <c r="G5" t="s">
-        <v>175</v>
-      </c>
-      <c r="H5" t="s">
-        <v>176</v>
-      </c>
-      <c r="I5" t="s">
-        <v>177</v>
+        <v>138</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>170</v>
+        <v>101</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B10" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B12" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="B14" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B15" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>127</v>
-      </c>
-      <c r="B17" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>128</v>
-      </c>
-      <c r="B18" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>186</v>
-      </c>
-      <c r="B19" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>188</v>
-      </c>
-      <c r="B20" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>190</v>
-      </c>
-      <c r="B21" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>192</v>
-      </c>
-      <c r="B22" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>194</v>
-      </c>
-      <c r="B23" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>196</v>
-      </c>
-      <c r="B24" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>198</v>
-      </c>
-      <c r="B25" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>200</v>
-      </c>
-      <c r="B26" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>202</v>
-      </c>
-      <c r="B27" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>204</v>
-      </c>
-      <c r="B28" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>206</v>
-      </c>
-      <c r="B29" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>208</v>
-      </c>
-      <c r="B30" t="s">
-        <v>209</v>
       </c>
     </row>
   </sheetData>
@@ -3704,7 +3653,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="J2" activeCellId="1" sqref="B2:B9 J2:J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3838,4 +3787,246 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABCFE19-EE98-9640-BD27-491E18EEB14A}">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C10" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>207</v>
+      </c>
+      <c r="B11" t="s">
+        <v>165</v>
+      </c>
+      <c r="C11" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>208</v>
+      </c>
+      <c r="B12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B13" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>210</v>
+      </c>
+      <c r="B14" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>211</v>
+      </c>
+      <c r="B15" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>213</v>
+      </c>
+      <c r="B17" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>214</v>
+      </c>
+      <c r="B18" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B19" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>216</v>
+      </c>
+      <c r="B20" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>217</v>
+      </c>
+      <c r="B21" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>126</v>
+      </c>
+      <c r="B22" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" t="s">
+        <v>197</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
axe unused loc data from tourney sheets
</commit_message>
<xml_diff>
--- a/src/stp/database/2018-mens-world-cup.xlsx
+++ b/src/stp/database/2018-mens-world-cup.xlsx
@@ -8,16 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/src/stp/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB5F5D5-86DF-534F-B543-D0BDF358132F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C321CA35-153D-E644-BFF3-CE3AF49C743A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19280" activeTab="4" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19280" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tournament" sheetId="8" r:id="rId1"/>
+    <sheet name="Properties" sheetId="10" r:id="rId1"/>
     <sheet name="Matches" sheetId="1" r:id="rId2"/>
     <sheet name="Seeds" sheetId="3" r:id="rId3"/>
-    <sheet name="Colors" sheetId="9" r:id="rId4"/>
-    <sheet name="Properties" sheetId="10" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="166">
   <si>
     <t>A1</t>
   </si>
@@ -237,9 +235,6 @@
     <t>venue</t>
   </si>
   <si>
-    <t>location</t>
-  </si>
-  <si>
     <t>seed</t>
   </si>
   <si>
@@ -324,54 +319,6 @@
     <t>key</t>
   </si>
   <si>
-    <t>en</t>
-  </si>
-  <si>
-    <t>es</t>
-  </si>
-  <si>
-    <t>fr</t>
-  </si>
-  <si>
-    <t>it</t>
-  </si>
-  <si>
-    <t>de</t>
-  </si>
-  <si>
-    <t>nl</t>
-  </si>
-  <si>
-    <t>venue.1</t>
-  </si>
-  <si>
-    <t>venue.2</t>
-  </si>
-  <si>
-    <t>venue.3</t>
-  </si>
-  <si>
-    <t>venue.4</t>
-  </si>
-  <si>
-    <t>venue.5</t>
-  </si>
-  <si>
-    <t>venue.6</t>
-  </si>
-  <si>
-    <t>venue.7</t>
-  </si>
-  <si>
-    <t>venue.8</t>
-  </si>
-  <si>
-    <t>fa</t>
-  </si>
-  <si>
-    <t>ja</t>
-  </si>
-  <si>
     <t>home-score</t>
   </si>
   <si>
@@ -384,9 +331,6 @@
     <t>home-tiebreaker</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>team</t>
   </si>
   <si>
@@ -414,12 +358,6 @@
     <t>COL</t>
   </si>
   <si>
-    <t>Russia</t>
-  </si>
-  <si>
-    <t>venue.9</t>
-  </si>
-  <si>
     <t>venue.10</t>
   </si>
   <si>
@@ -429,42 +367,6 @@
     <t>venue.12</t>
   </si>
   <si>
-    <t>Ekaterinburg Stadium</t>
-  </si>
-  <si>
-    <t>Saint Petersburg Stadium</t>
-  </si>
-  <si>
-    <t>Kazan Arena</t>
-  </si>
-  <si>
-    <t>Saransk Stadium</t>
-  </si>
-  <si>
-    <t>Kaliningrad Stadium</t>
-  </si>
-  <si>
-    <t>Samara Stadium</t>
-  </si>
-  <si>
-    <t>Rostov-on-Don Stadium</t>
-  </si>
-  <si>
-    <t>Nizhny Novgorod Stadium</t>
-  </si>
-  <si>
-    <t>Volgograd Stadium</t>
-  </si>
-  <si>
-    <t>Luzhniki Stadium</t>
-  </si>
-  <si>
-    <t>Fisht Stadium</t>
-  </si>
-  <si>
-    <t>Otkrytiye Arena</t>
-  </si>
-  <si>
     <t>home-team</t>
   </si>
   <si>
@@ -480,124 +382,34 @@
     <t>notes</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>#94d9f5</t>
   </si>
   <si>
-    <t>pale cyan</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>#fee289</t>
   </si>
   <si>
-    <t>pale yellow</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>#f79d8f</t>
   </si>
   <si>
-    <t>pale red</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>#c4e1b5</t>
   </si>
   <si>
-    <t>pale green</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
     <t>#b0d0ee</t>
   </si>
   <si>
-    <t>pale blue</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
     <t>#c0e4df</t>
   </si>
   <si>
-    <t>pale teal</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
     <t>#fab077</t>
   </si>
   <si>
-    <t>pale orange</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>#eecbef</t>
   </si>
   <si>
-    <t>pale purple</t>
-  </si>
-  <si>
     <t>timezone</t>
   </si>
   <si>
     <t>Europe/Moscow</t>
-  </si>
-  <si>
-    <t>Rusia</t>
-  </si>
-  <si>
-    <t>Russie</t>
-  </si>
-  <si>
-    <t>Russland</t>
-  </si>
-  <si>
-    <t>Rusland</t>
-  </si>
-  <si>
-    <t>ロシア</t>
-  </si>
-  <si>
-    <t>روسیه</t>
-  </si>
-  <si>
-    <t>World Cup</t>
-  </si>
-  <si>
-    <t>Copa del Mundo</t>
-  </si>
-  <si>
-    <t>Coppa del Mondo</t>
-  </si>
-  <si>
-    <t>Coupe du monde</t>
-  </si>
-  <si>
-    <t>Weltmeisterschaft</t>
-  </si>
-  <si>
-    <t>Wereldkampioenschap</t>
-  </si>
-  <si>
-    <t>W杯</t>
-  </si>
-  <si>
-    <t>جام جهانی</t>
   </si>
   <si>
     <t>ru-moscow_luzhniki</t>
@@ -730,7 +542,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -743,12 +555,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -771,18 +577,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="8">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -821,18 +623,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{A35F1197-A800-47A7-9FB8-27BA1E42FC3F}" name="tournament" displayName="tournament" ref="A1:I16" totalsRowShown="0">
-  <autoFilter ref="A1:I16" xr:uid="{A35F1197-A800-47A7-9FB8-27BA1E42FC3F}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{A8CDEDD3-FA49-4AD4-8D9F-D3DFCABC2052}" name="key"/>
-    <tableColumn id="2" xr3:uid="{88778009-1F1A-4B0F-BCE2-A71F4DD7CF67}" name="en"/>
-    <tableColumn id="3" xr3:uid="{B0854098-6051-4EC6-B153-6F15A5D8EDE3}" name="es"/>
-    <tableColumn id="4" xr3:uid="{451E0539-ECF2-4BD5-A71E-337F41B0AED7}" name="it"/>
-    <tableColumn id="5" xr3:uid="{B50399C0-B1D0-4B7B-9997-0B86C7572F77}" name="fr"/>
-    <tableColumn id="6" xr3:uid="{B0F7BA24-53BA-4D61-BC1C-8F39E4CFC9AD}" name="de"/>
-    <tableColumn id="7" xr3:uid="{F2DB2A1A-9388-4CD2-9231-4B516407345F}" name="nl"/>
-    <tableColumn id="8" xr3:uid="{E069B466-BE62-49FE-858B-990B30F1EE20}" name="ja"/>
-    <tableColumn id="9" xr3:uid="{29A41F5D-C82C-4A8F-B732-857BFD0D7766}" name="fa"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AEEE4923-055B-A14A-9B48-3E0283A1160B}" name="Properties" displayName="Properties" ref="A1:C24" totalsRowShown="0">
+  <autoFilter ref="A1:C24" xr:uid="{AEEE4923-055B-A14A-9B48-3E0283A1160B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C24">
+    <sortCondition ref="A1:A24"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{31E242A4-4364-304E-A4A7-4443C29CFCC1}" name="key"/>
+    <tableColumn id="2" xr3:uid="{7AFBD417-707A-F242-BB43-CEC5BB264EDA}" name="value"/>
+    <tableColumn id="3" xr3:uid="{4306B17E-8C36-1A4B-BF13-4EB899EF33B6}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -845,14 +644,14 @@
     <tableColumn id="1" xr3:uid="{35D3E9F5-BB3B-4940-9EB6-C927FD84875C}" name="match"/>
     <tableColumn id="2" xr3:uid="{97337EE3-AAC3-4452-8381-1A56C6B35138}" name="home-seed"/>
     <tableColumn id="3" xr3:uid="{AEDB8750-5B25-4357-9054-E49FECC94717}" name="away-seed"/>
-    <tableColumn id="4" xr3:uid="{B178F43D-E631-4314-9E59-2CDA6EDA94F1}" name="time" dataDxfId="8"/>
-    <tableColumn id="16" xr3:uid="{398EE86D-DB71-4B07-BCF3-5E13F225DA53}" name="venue" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{68E01095-6C68-42AF-8716-32FC9C3B5D8B}" name="home-team" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{2CDCD506-6640-41AE-846E-162E81849C6B}" name="away-team" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{B178F43D-E631-4314-9E59-2CDA6EDA94F1}" name="time" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{398EE86D-DB71-4B07-BCF3-5E13F225DA53}" name="venue" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{68E01095-6C68-42AF-8716-32FC9C3B5D8B}" name="home-team" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{2CDCD506-6640-41AE-846E-162E81849C6B}" name="away-team" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -864,40 +663,6 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{C0AEBB99-51D0-46B6-ACD7-C4F2DC461A4C}" name="seed"/>
     <tableColumn id="3" xr3:uid="{DD8C8688-8EED-4B48-9C61-D766CD3EFBBB}" name="team"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9D90DA66-9083-46D7-BA4F-82B790147407}" name="groups" displayName="groups" ref="A1:J9" totalsRowShown="0">
-  <autoFilter ref="A1:J9" xr:uid="{4B86982E-77B7-4963-838F-4D594C24841B}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{88EE909C-168A-4B2F-B567-03E45EA308EE}" name="key"/>
-    <tableColumn id="2" xr3:uid="{9507E86E-E495-4A60-A1C2-B22B68769689}" name="en"/>
-    <tableColumn id="3" xr3:uid="{C9200991-F3E3-4176-89AD-04BCE044B1C6}" name="es"/>
-    <tableColumn id="4" xr3:uid="{1C7242BE-C401-4B86-9194-9D006617A6C1}" name="it"/>
-    <tableColumn id="5" xr3:uid="{2AF12BA5-BC5B-491C-88CA-D0E57D581F16}" name="fr"/>
-    <tableColumn id="6" xr3:uid="{1D61E46B-3B2C-4922-9B65-C97BF9F3EF2D}" name="de"/>
-    <tableColumn id="7" xr3:uid="{6243B05C-6BAE-4D3D-9B50-8E8C73F0BCD4}" name="nl"/>
-    <tableColumn id="8" xr3:uid="{6119E755-9CCC-4ABE-99D9-63CBF4D891CB}" name="ja"/>
-    <tableColumn id="9" xr3:uid="{12D54549-EC84-4A42-ACAB-B413320B4F44}" name="fa" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{1AF993A1-3EBC-4103-B829-4C6FDE197432}" name="notes"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{AEEE4923-055B-A14A-9B48-3E0283A1160B}" name="Properties" displayName="Properties" ref="A1:C24" totalsRowShown="0">
-  <autoFilter ref="A1:C24" xr:uid="{AEEE4923-055B-A14A-9B48-3E0283A1160B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C24">
-    <sortCondition ref="A1:A24"/>
-  </sortState>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{31E242A4-4364-304E-A4A7-4443C29CFCC1}" name="key"/>
-    <tableColumn id="2" xr3:uid="{7AFBD417-707A-F242-BB43-CEC5BB264EDA}" name="value"/>
-    <tableColumn id="3" xr3:uid="{4306B17E-8C36-1A4B-BF13-4EB899EF33B6}" name="notes"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1199,226 +964,243 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393FFACE-29F0-47F7-B7AD-389E0D6667C5}">
-  <dimension ref="A1:I16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABCFE19-EE98-9640-BD27-491E18EEB14A}">
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17:XFD28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>138</v>
       </c>
       <c r="C1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C12" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>155</v>
+      </c>
+      <c r="B21" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>107</v>
+      </c>
+      <c r="B23" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" t="s">
-        <v>178</v>
-      </c>
-      <c r="C2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E2" t="s">
-        <v>181</v>
-      </c>
-      <c r="F2" t="s">
-        <v>182</v>
-      </c>
-      <c r="G2" t="s">
-        <v>183</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="I2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F3" t="s">
-        <v>174</v>
-      </c>
-      <c r="G3" t="s">
-        <v>175</v>
-      </c>
-      <c r="H3" t="s">
-        <v>176</v>
-      </c>
-      <c r="I3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>101</v>
-      </c>
-      <c r="B6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B8" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>104</v>
-      </c>
-      <c r="B9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>105</v>
-      </c>
-      <c r="B10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>107</v>
-      </c>
-      <c r="B12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>125</v>
-      </c>
-      <c r="B13" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="B24" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>127</v>
-      </c>
-      <c r="B15" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>128</v>
-      </c>
-      <c r="B16" t="s">
-        <v>137</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1446,10 +1228,10 @@
         <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>143</v>
+        <v>111</v>
       </c>
       <c r="C1" t="s">
-        <v>144</v>
+        <v>112</v>
       </c>
       <c r="D1" t="s">
         <v>63</v>
@@ -1458,22 +1240,22 @@
         <v>64</v>
       </c>
       <c r="F1" t="s">
-        <v>141</v>
+        <v>109</v>
       </c>
       <c r="G1" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
       <c r="H1" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="I1" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="J1" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="K1" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -1493,10 +1275,10 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="G2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H2">
         <v>5</v>
@@ -1522,10 +1304,10 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="G3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -1551,10 +1333,10 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H4">
         <v>3</v>
@@ -1580,10 +1362,10 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" t="s">
         <v>88</v>
-      </c>
-      <c r="G5" t="s">
-        <v>89</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1609,10 +1391,10 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6">
         <v>2</v>
@@ -1638,10 +1420,10 @@
         <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="G7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1667,10 +1449,10 @@
         <v>6</v>
       </c>
       <c r="F8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G8" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1696,10 +1478,10 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G9" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="H9">
         <v>2</v>
@@ -1725,10 +1507,10 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -1754,10 +1536,10 @@
         <v>9</v>
       </c>
       <c r="F11" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" t="s">
         <v>86</v>
-      </c>
-      <c r="G11" t="s">
-        <v>87</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1783,10 +1565,10 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -1812,10 +1594,10 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="G13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -1841,10 +1623,10 @@
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G14" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="H14">
         <v>3</v>
@@ -1870,10 +1652,10 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -1899,10 +1681,10 @@
         <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -1928,10 +1710,10 @@
         <v>7</v>
       </c>
       <c r="F17" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="G17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -1957,10 +1739,10 @@
         <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="G18" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="H18">
         <v>3</v>
@@ -1986,10 +1768,10 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H19">
         <v>1</v>
@@ -2015,10 +1797,10 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H20">
         <v>1</v>
@@ -2044,10 +1826,10 @@
         <v>5</v>
       </c>
       <c r="F21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -2073,10 +1855,10 @@
         <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G22" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="H22">
         <v>1</v>
@@ -2102,10 +1884,10 @@
         <v>9</v>
       </c>
       <c r="F23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H23">
         <v>1</v>
@@ -2131,10 +1913,10 @@
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -2160,10 +1942,10 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="G25" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="H25">
         <v>2</v>
@@ -2189,10 +1971,10 @@
         <v>3</v>
       </c>
       <c r="F26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H26">
         <v>2</v>
@@ -2218,10 +2000,10 @@
         <v>8</v>
       </c>
       <c r="F27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H27">
         <v>1</v>
@@ -2247,10 +2029,10 @@
         <v>4</v>
       </c>
       <c r="F28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G28" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="H28">
         <v>2</v>
@@ -2276,10 +2058,10 @@
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H29">
         <v>1</v>
@@ -2305,10 +2087,10 @@
         <v>6</v>
       </c>
       <c r="F30" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H30">
         <v>5</v>
@@ -2334,10 +2116,10 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G31" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="H31">
         <v>6</v>
@@ -2363,10 +2145,10 @@
         <v>5</v>
       </c>
       <c r="F32" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G32" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -2392,10 +2174,10 @@
         <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H33">
         <v>2</v>
@@ -2421,10 +2203,10 @@
         <v>9</v>
       </c>
       <c r="F34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G34" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="H34">
         <v>3</v>
@@ -2450,10 +2232,10 @@
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G35" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="H35">
         <v>2</v>
@@ -2479,10 +2261,10 @@
         <v>7</v>
       </c>
       <c r="F36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G36" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H36">
         <v>1</v>
@@ -2508,10 +2290,10 @@
         <v>8</v>
       </c>
       <c r="F37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H37">
         <v>2</v>
@@ -2537,10 +2319,10 @@
         <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G38" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -2566,10 +2348,10 @@
         <v>4</v>
       </c>
       <c r="F39" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G39" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -2595,10 +2377,10 @@
         <v>3</v>
       </c>
       <c r="F40" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
       <c r="G40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H40">
         <v>1</v>
@@ -2624,10 +2406,10 @@
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
       <c r="G41" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H41">
         <v>1</v>
@@ -2653,10 +2435,10 @@
         <v>6</v>
       </c>
       <c r="F42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -2682,10 +2464,10 @@
         <v>1</v>
       </c>
       <c r="F43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G43" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H43">
         <v>2</v>
@@ -2711,10 +2493,10 @@
         <v>5</v>
       </c>
       <c r="F44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H44">
         <v>2</v>
@@ -2740,10 +2522,10 @@
         <v>2</v>
       </c>
       <c r="F45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G45" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -2769,10 +2551,10 @@
         <v>8</v>
       </c>
       <c r="F46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G46" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -2798,10 +2580,10 @@
         <v>7</v>
       </c>
       <c r="F47" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="G47" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H47">
         <v>1</v>
@@ -2827,10 +2609,10 @@
         <v>1</v>
       </c>
       <c r="F48" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -2856,10 +2638,10 @@
         <v>9</v>
       </c>
       <c r="F49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G49" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -2885,10 +2667,10 @@
         <v>4</v>
       </c>
       <c r="F50" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G50" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H50">
         <v>2</v>
@@ -2914,10 +2696,10 @@
         <v>5</v>
       </c>
       <c r="F51" t="s">
+        <v>68</v>
+      </c>
+      <c r="G51" t="s">
         <v>69</v>
-      </c>
-      <c r="G51" t="s">
-        <v>70</v>
       </c>
       <c r="H51">
         <v>4</v>
@@ -2943,10 +2725,10 @@
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G52" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="H52">
         <v>1</v>
@@ -2978,10 +2760,10 @@
         <v>1</v>
       </c>
       <c r="F53" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G53" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H53">
         <v>1</v>
@@ -3013,10 +2795,10 @@
         <v>9</v>
       </c>
       <c r="F54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H54">
         <v>2</v>
@@ -3042,10 +2824,10 @@
         <v>1</v>
       </c>
       <c r="F55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H55">
         <v>3</v>
@@ -3071,10 +2853,10 @@
         <v>3</v>
       </c>
       <c r="F56" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="G56" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H56">
         <v>1</v>
@@ -3100,10 +2882,10 @@
         <v>6</v>
       </c>
       <c r="F57" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="G57" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H57">
         <v>1</v>
@@ -3135,10 +2917,10 @@
         <v>1</v>
       </c>
       <c r="F58" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G58" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -3164,10 +2946,10 @@
         <v>5</v>
       </c>
       <c r="F59" t="s">
+        <v>66</v>
+      </c>
+      <c r="G59" t="s">
         <v>67</v>
-      </c>
-      <c r="G59" t="s">
-        <v>68</v>
       </c>
       <c r="H59">
         <v>1</v>
@@ -3193,10 +2975,10 @@
         <v>4</v>
       </c>
       <c r="F60" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="G60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H60">
         <v>2</v>
@@ -3228,10 +3010,10 @@
         <v>9</v>
       </c>
       <c r="F61" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
       <c r="G61" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -3257,10 +3039,10 @@
         <v>3</v>
       </c>
       <c r="F62" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G62" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H62">
         <v>1</v>
@@ -3286,10 +3068,10 @@
         <v>1</v>
       </c>
       <c r="F63" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G63" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H63">
         <v>2</v>
@@ -3303,10 +3085,10 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
+        <v>90</v>
+      </c>
+      <c r="C64" t="s">
         <v>91</v>
-      </c>
-      <c r="C64" t="s">
-        <v>92</v>
       </c>
       <c r="D64" s="1">
         <v>43295.583333333336</v>
@@ -3315,10 +3097,10 @@
         <v>3</v>
       </c>
       <c r="F64" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G64" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H64">
         <v>2</v>
@@ -3344,10 +3126,10 @@
         <v>1</v>
       </c>
       <c r="F65" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H65">
         <v>4</v>
@@ -3377,10 +3159,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -3388,7 +3170,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3396,7 +3178,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -3404,7 +3186,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -3412,7 +3194,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -3420,7 +3202,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3428,7 +3210,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -3436,7 +3218,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3444,7 +3226,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -3452,7 +3234,7 @@
         <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -3460,7 +3242,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
@@ -3468,7 +3250,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -3476,7 +3258,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
@@ -3484,7 +3266,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -3492,7 +3274,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
@@ -3500,7 +3282,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
@@ -3508,7 +3290,7 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
@@ -3516,7 +3298,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
@@ -3524,7 +3306,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -3532,7 +3314,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
@@ -3540,7 +3322,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -3548,7 +3330,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -3556,7 +3338,7 @@
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
@@ -3564,7 +3346,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
@@ -3572,7 +3354,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
@@ -3580,7 +3362,7 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
@@ -3588,7 +3370,7 @@
         <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
@@ -3596,7 +3378,7 @@
         <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
@@ -3604,7 +3386,7 @@
         <v>25</v>
       </c>
       <c r="B29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
@@ -3612,7 +3394,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
@@ -3620,7 +3402,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
@@ -3628,7 +3410,7 @@
         <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -3636,7 +3418,7 @@
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -3646,387 +3428,4 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC88D2E7-F4E0-42E8-919E-CAB4A74488F8}">
-  <dimension ref="A1:J9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" activeCellId="1" sqref="B2:B9 J2:J9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" t="s">
-        <v>97</v>
-      </c>
-      <c r="E1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H1" t="s">
-        <v>109</v>
-      </c>
-      <c r="I1" t="s">
-        <v>108</v>
-      </c>
-      <c r="J1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>146</v>
-      </c>
-      <c r="B2" t="s">
-        <v>147</v>
-      </c>
-      <c r="J2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B3" t="s">
-        <v>150</v>
-      </c>
-      <c r="J3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>152</v>
-      </c>
-      <c r="B4" t="s">
-        <v>153</v>
-      </c>
-      <c r="J4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B5" t="s">
-        <v>156</v>
-      </c>
-      <c r="J5" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>158</v>
-      </c>
-      <c r="B6" t="s">
-        <v>159</v>
-      </c>
-      <c r="J6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>161</v>
-      </c>
-      <c r="B7" t="s">
-        <v>162</v>
-      </c>
-      <c r="J7" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>164</v>
-      </c>
-      <c r="B8" t="s">
-        <v>165</v>
-      </c>
-      <c r="J8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>167</v>
-      </c>
-      <c r="B9" t="s">
-        <v>168</v>
-      </c>
-      <c r="J9" t="s">
-        <v>169</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABCFE19-EE98-9640-BD27-491E18EEB14A}">
-  <dimension ref="A1:C24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" t="s">
-        <v>200</v>
-      </c>
-      <c r="C1" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>218</v>
-      </c>
-      <c r="B2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>219</v>
-      </c>
-      <c r="B3" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>170</v>
-      </c>
-      <c r="B4" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>201</v>
-      </c>
-      <c r="B5" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>202</v>
-      </c>
-      <c r="B6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C6" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>203</v>
-      </c>
-      <c r="B7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C7" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>204</v>
-      </c>
-      <c r="B8" t="s">
-        <v>156</v>
-      </c>
-      <c r="C8" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>205</v>
-      </c>
-      <c r="B9" t="s">
-        <v>159</v>
-      </c>
-      <c r="C9" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>206</v>
-      </c>
-      <c r="B10" t="s">
-        <v>162</v>
-      </c>
-      <c r="C10" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>207</v>
-      </c>
-      <c r="B11" t="s">
-        <v>165</v>
-      </c>
-      <c r="C11" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>208</v>
-      </c>
-      <c r="B12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C12" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>209</v>
-      </c>
-      <c r="B13" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>210</v>
-      </c>
-      <c r="B14" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>211</v>
-      </c>
-      <c r="B15" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>212</v>
-      </c>
-      <c r="B16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>213</v>
-      </c>
-      <c r="B17" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>214</v>
-      </c>
-      <c r="B18" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>215</v>
-      </c>
-      <c r="B19" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>216</v>
-      </c>
-      <c r="B20" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>217</v>
-      </c>
-      <c r="B21" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>126</v>
-      </c>
-      <c r="B22" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>127</v>
-      </c>
-      <c r="B23" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>128</v>
-      </c>
-      <c r="B24" t="s">
-        <v>197</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
corrected results (via knockout round visualizations)
</commit_message>
<xml_diff>
--- a/src/stp/database/2018-mens-world-cup.xlsx
+++ b/src/stp/database/2018-mens-world-cup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/src/stp/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C321CA35-153D-E644-BFF3-CE3AF49C743A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF356C4-47D3-9944-A31D-363CA1D219E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19280" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19280" activeTab="1" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="10" r:id="rId1"/>
@@ -967,7 +967,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABCFE19-EE98-9640-BD27-491E18EEB14A}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
@@ -1209,8 +1209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ABE575-0207-4299-82CD-74F27B6194DA}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2963,10 +2963,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C60" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D60" s="1">
         <v>43288.75</v>
@@ -2998,10 +2998,10 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C61" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D61" s="1">
         <v>43288.583333333336</v>

</xml_diff>

<commit_message>
cleaned 2018 sheet for 2nd claude fill in attempt
</commit_message>
<xml_diff>
--- a/src/stp/database/2018-mens-world-cup.xlsx
+++ b/src/stp/database/2018-mens-world-cup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bruceoberg/code/soccer-tourney-poster/src/stp/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF356C4-47D3-9944-A31D-363CA1D219E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDB53639-30AC-A944-A3D3-4EE0E026B355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="38400" windowHeight="19280" activeTab="1" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="34200" windowHeight="19280" activeTab="1" xr2:uid="{51C3DE88-701F-4CAC-8963-452186F7FFBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Properties" sheetId="10" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="169">
   <si>
     <t>A1</t>
   </si>
@@ -536,6 +536,15 @@
   </si>
   <si>
     <t>purple</t>
+  </si>
+  <si>
+    <t>home-known</t>
+  </si>
+  <si>
+    <t>away-known</t>
+  </si>
+  <si>
+    <t>after-extra-time</t>
   </si>
 </sst>
 </file>
@@ -584,7 +593,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -638,20 +653,27 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D36B1D81-AA68-4E33-AA36-B206B4FF7406}" name="matches" displayName="matches" ref="A1:K65" totalsRowShown="0">
-  <autoFilter ref="A1:K65" xr:uid="{D36B1D81-AA68-4E33-AA36-B206B4FF7406}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D36B1D81-AA68-4E33-AA36-B206B4FF7406}" name="matches" displayName="matches" ref="A1:N65" totalsRowShown="0">
+  <autoFilter ref="A1:N65" xr:uid="{D36B1D81-AA68-4E33-AA36-B206B4FF7406}"/>
+  <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{35D3E9F5-BB3B-4940-9EB6-C927FD84875C}" name="match"/>
     <tableColumn id="2" xr3:uid="{97337EE3-AAC3-4452-8381-1A56C6B35138}" name="home-seed"/>
     <tableColumn id="3" xr3:uid="{AEDB8750-5B25-4357-9054-E49FECC94717}" name="away-seed"/>
-    <tableColumn id="4" xr3:uid="{B178F43D-E631-4314-9E59-2CDA6EDA94F1}" name="time" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{398EE86D-DB71-4B07-BCF3-5E13F225DA53}" name="venue" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{68E01095-6C68-42AF-8716-32FC9C3B5D8B}" name="home-team" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{2CDCD506-6640-41AE-846E-162E81849C6B}" name="away-team" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{B178F43D-E631-4314-9E59-2CDA6EDA94F1}" name="time" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{398EE86D-DB71-4B07-BCF3-5E13F225DA53}" name="venue" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{D328D66C-B736-FF4F-98AD-5A287ED0BDA2}" name="home-known" dataDxfId="1">
+      <calculatedColumnFormula>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{09952783-0B36-F342-A78C-BE91C6DC01DF}" name="away-known" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="11" xr3:uid="{68E01095-6C68-42AF-8716-32FC9C3B5D8B}" name="home-team" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{2CDCD506-6640-41AE-846E-162E81849C6B}" name="away-team" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{A0CDBBB6-1128-45BC-8300-89FE399860C1}" name="home-score" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{95DA1082-F87D-4A64-B45A-77AEEA888386}" name="away-score" dataDxfId="4"/>
+    <tableColumn id="14" xr3:uid="{06CE9C18-71B8-0F4E-ACAF-25BC22F0E0E5}" name="after-extra-time"/>
+    <tableColumn id="8" xr3:uid="{5865175D-2339-4B50-A707-595597D0BEF5}" name="home-tiebreaker" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{967E27DF-151D-40C4-9623-59691A5D7311}" name="away-tiebreaker" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1207,23 +1229,31 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2ABE575-0207-4299-82CD-74F27B6194DA}">
-  <dimension ref="A1:K65"/>
+  <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.1640625" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>62</v>
       </c>
@@ -1240,25 +1270,34 @@
         <v>64</v>
       </c>
       <c r="F1" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" t="s">
         <v>109</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>110</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>93</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>94</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
+        <v>168</v>
+      </c>
+      <c r="M1" t="s">
         <v>96</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1274,20 +1313,16 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>98</v>
-      </c>
-      <c r="G2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H2">
-        <v>5</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F2" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>RUS</v>
+      </c>
+      <c r="G2" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>KSA</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1303,20 +1338,16 @@
       <c r="E3">
         <v>2</v>
       </c>
-      <c r="F3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F3" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>EGY</v>
+      </c>
+      <c r="G3" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>URU</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1332,20 +1363,16 @@
       <c r="E4">
         <v>4</v>
       </c>
-      <c r="F4" t="s">
-        <v>71</v>
-      </c>
-      <c r="G4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F4" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>MAR</v>
+      </c>
+      <c r="G4" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>IRN</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1361,20 +1388,16 @@
       <c r="E5">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
-        <v>87</v>
-      </c>
-      <c r="G5" t="s">
-        <v>88</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F5" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>POR</v>
+      </c>
+      <c r="G5" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>ESP</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1390,20 +1413,16 @@
       <c r="E6">
         <v>5</v>
       </c>
-      <c r="F6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" t="s">
-        <v>79</v>
-      </c>
-      <c r="H6">
-        <v>2</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F6" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>FRA</v>
+      </c>
+      <c r="G6" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>AUS</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1419,20 +1438,16 @@
       <c r="E7">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
-        <v>100</v>
-      </c>
-      <c r="G7" t="s">
-        <v>73</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F7" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>ARG</v>
+      </c>
+      <c r="G7" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>ISL</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1448,20 +1463,16 @@
       <c r="E8">
         <v>6</v>
       </c>
-      <c r="F8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F8" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>PER</v>
+      </c>
+      <c r="G8" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>DEN</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1477,20 +1488,16 @@
       <c r="E9">
         <v>8</v>
       </c>
-      <c r="F9" t="s">
-        <v>76</v>
-      </c>
-      <c r="G9" t="s">
-        <v>102</v>
-      </c>
-      <c r="H9">
-        <v>2</v>
-      </c>
-      <c r="I9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F9" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>CRO</v>
+      </c>
+      <c r="G9" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>NGA</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1506,20 +1513,16 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" t="s">
-        <v>66</v>
-      </c>
-      <c r="G10" t="s">
-        <v>82</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F10" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>CRC</v>
+      </c>
+      <c r="G10" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>SRB</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1535,20 +1538,16 @@
       <c r="E11">
         <v>9</v>
       </c>
-      <c r="F11" t="s">
-        <v>85</v>
-      </c>
-      <c r="G11" t="s">
-        <v>86</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F11" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>GER</v>
+      </c>
+      <c r="G11" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>MEX</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1564,20 +1563,16 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" t="s">
-        <v>72</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F12" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>BRA</v>
+      </c>
+      <c r="G12" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>SUI</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1593,20 +1588,16 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13" t="s">
-        <v>103</v>
-      </c>
-      <c r="G13" t="s">
-        <v>84</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F13" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>SWE</v>
+      </c>
+      <c r="G13" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>KOR</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1622,20 +1613,16 @@
       <c r="E14">
         <v>4</v>
       </c>
-      <c r="F14" t="s">
-        <v>67</v>
-      </c>
-      <c r="G14" t="s">
-        <v>104</v>
-      </c>
-      <c r="H14">
-        <v>3</v>
-      </c>
-      <c r="I14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F14" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>BEL</v>
+      </c>
+      <c r="G14" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>PAN</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1651,20 +1638,16 @@
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15" t="s">
-        <v>80</v>
-      </c>
-      <c r="G15" t="s">
-        <v>70</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F15" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>TUN</v>
+      </c>
+      <c r="G15" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>ENG</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1680,20 +1663,16 @@
       <c r="E16">
         <v>6</v>
       </c>
-      <c r="F16" t="s">
-        <v>78</v>
-      </c>
-      <c r="G16" t="s">
-        <v>77</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-      <c r="I16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F16" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>COL</v>
+      </c>
+      <c r="G16" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>JPN</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1709,20 +1688,16 @@
       <c r="E17">
         <v>7</v>
       </c>
-      <c r="F17" t="s">
-        <v>105</v>
-      </c>
-      <c r="G17" t="s">
-        <v>83</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-      <c r="I17">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F17" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>POL</v>
+      </c>
+      <c r="G17" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>SEN</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1738,20 +1713,16 @@
       <c r="E18">
         <v>3</v>
       </c>
-      <c r="F18" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" t="s">
-        <v>99</v>
-      </c>
-      <c r="H18">
-        <v>3</v>
-      </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F18" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>RUS</v>
+      </c>
+      <c r="G18" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>EGY</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1767,20 +1738,16 @@
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" t="s">
-        <v>89</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F19" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>POR</v>
+      </c>
+      <c r="G19" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>MAR</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1796,20 +1763,16 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20" t="s">
-        <v>71</v>
-      </c>
-      <c r="G20" t="s">
-        <v>87</v>
-      </c>
-      <c r="H20">
-        <v>1</v>
-      </c>
-      <c r="I20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F20" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>URU</v>
+      </c>
+      <c r="G20" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>KSA</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1825,20 +1788,16 @@
       <c r="E21">
         <v>5</v>
       </c>
-      <c r="F21" t="s">
-        <v>88</v>
-      </c>
-      <c r="G21" t="s">
-        <v>81</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F21" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>IRN</v>
+      </c>
+      <c r="G21" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>ESP</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1854,20 +1813,16 @@
       <c r="E22">
         <v>2</v>
       </c>
-      <c r="F22" t="s">
-        <v>68</v>
-      </c>
-      <c r="G22" t="s">
-        <v>100</v>
-      </c>
-      <c r="H22">
-        <v>1</v>
-      </c>
-      <c r="I22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F22" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>DEN</v>
+      </c>
+      <c r="G22" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>AUS</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1883,20 +1838,16 @@
       <c r="E23">
         <v>9</v>
       </c>
-      <c r="F23" t="s">
-        <v>73</v>
-      </c>
-      <c r="G23" t="s">
-        <v>79</v>
-      </c>
-      <c r="H23">
-        <v>1</v>
-      </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F23" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>FRA</v>
+      </c>
+      <c r="G23" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>PER</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1912,20 +1863,16 @@
       <c r="E24">
         <v>1</v>
       </c>
-      <c r="F24" t="s">
-        <v>69</v>
-      </c>
-      <c r="G24" t="s">
-        <v>76</v>
-      </c>
-      <c r="H24">
-        <v>0</v>
-      </c>
-      <c r="I24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F24" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>ARG</v>
+      </c>
+      <c r="G24" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>CRO</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1941,20 +1888,16 @@
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25" t="s">
-        <v>102</v>
-      </c>
-      <c r="G25" t="s">
-        <v>101</v>
-      </c>
-      <c r="H25">
-        <v>2</v>
-      </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F25" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>BRA</v>
+      </c>
+      <c r="G25" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>CRC</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1970,20 +1913,16 @@
       <c r="E26">
         <v>3</v>
       </c>
-      <c r="F26" t="s">
-        <v>66</v>
-      </c>
-      <c r="G26" t="s">
-        <v>85</v>
-      </c>
-      <c r="H26">
-        <v>2</v>
-      </c>
-      <c r="I26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F26" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>NGA</v>
+      </c>
+      <c r="G26" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>ISL</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1999,20 +1938,16 @@
       <c r="E27">
         <v>8</v>
       </c>
-      <c r="F27" t="s">
-        <v>86</v>
-      </c>
-      <c r="G27" t="s">
-        <v>82</v>
-      </c>
-      <c r="H27">
-        <v>1</v>
-      </c>
-      <c r="I27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F27" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>SRB</v>
+      </c>
+      <c r="G27" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>SUI</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2028,20 +1963,16 @@
       <c r="E28">
         <v>4</v>
       </c>
-      <c r="F28" t="s">
-        <v>74</v>
-      </c>
-      <c r="G28" t="s">
-        <v>103</v>
-      </c>
-      <c r="H28">
-        <v>2</v>
-      </c>
-      <c r="I28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F28" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>BEL</v>
+      </c>
+      <c r="G28" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>TUN</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2057,20 +1988,16 @@
       <c r="E29">
         <v>1</v>
       </c>
-      <c r="F29" t="s">
-        <v>84</v>
-      </c>
-      <c r="G29" t="s">
-        <v>72</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-      <c r="I29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F29" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>KOR</v>
+      </c>
+      <c r="G29" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>MEX</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2086,20 +2013,16 @@
       <c r="E30">
         <v>6</v>
       </c>
-      <c r="F30" t="s">
-        <v>67</v>
-      </c>
-      <c r="G30" t="s">
-        <v>80</v>
-      </c>
-      <c r="H30">
-        <v>5</v>
-      </c>
-      <c r="I30">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F30" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>GER</v>
+      </c>
+      <c r="G30" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>SWE</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2115,20 +2038,16 @@
       <c r="E31">
         <v>1</v>
       </c>
-      <c r="F31" t="s">
-        <v>70</v>
-      </c>
-      <c r="G31" t="s">
-        <v>104</v>
-      </c>
-      <c r="H31">
-        <v>6</v>
-      </c>
-      <c r="I31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F31" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>ENG</v>
+      </c>
+      <c r="G31" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>PAN</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2144,20 +2063,16 @@
       <c r="E32">
         <v>5</v>
       </c>
-      <c r="F32" t="s">
-        <v>78</v>
-      </c>
-      <c r="G32" t="s">
-        <v>105</v>
-      </c>
-      <c r="H32">
-        <v>0</v>
-      </c>
-      <c r="I32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F32" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>JPN</v>
+      </c>
+      <c r="G32" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>SEN</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2173,20 +2088,16 @@
       <c r="E33">
         <v>2</v>
       </c>
-      <c r="F33" t="s">
-        <v>83</v>
-      </c>
-      <c r="G33" t="s">
-        <v>77</v>
-      </c>
-      <c r="H33">
-        <v>2</v>
-      </c>
-      <c r="I33">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F33" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>POL</v>
+      </c>
+      <c r="G33" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>COL</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2202,20 +2113,16 @@
       <c r="E34">
         <v>9</v>
       </c>
-      <c r="F34" t="s">
-        <v>75</v>
-      </c>
-      <c r="G34" t="s">
-        <v>98</v>
-      </c>
-      <c r="H34">
-        <v>3</v>
-      </c>
-      <c r="I34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F34" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>URU</v>
+      </c>
+      <c r="G34" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>RUS</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2231,20 +2138,16 @@
       <c r="E35">
         <v>1</v>
       </c>
-      <c r="F35" t="s">
-        <v>89</v>
-      </c>
-      <c r="G35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H35">
-        <v>2</v>
-      </c>
-      <c r="I35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F35" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>KSA</v>
+      </c>
+      <c r="G35" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>EGY</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2260,20 +2163,16 @@
       <c r="E36">
         <v>7</v>
       </c>
-      <c r="F36" t="s">
-        <v>88</v>
-      </c>
-      <c r="G36" t="s">
-        <v>71</v>
-      </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-      <c r="I36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F36" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>IRN</v>
+      </c>
+      <c r="G36" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>POR</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2289,20 +2188,16 @@
       <c r="E37">
         <v>8</v>
       </c>
-      <c r="F37" t="s">
-        <v>81</v>
-      </c>
-      <c r="G37" t="s">
-        <v>87</v>
-      </c>
-      <c r="H37">
-        <v>2</v>
-      </c>
-      <c r="I37">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F37" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>ESP</v>
+      </c>
+      <c r="G37" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>MAR</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2318,20 +2213,16 @@
       <c r="E38">
         <v>1</v>
       </c>
-      <c r="F38" t="s">
-        <v>73</v>
-      </c>
-      <c r="G38" t="s">
-        <v>68</v>
-      </c>
-      <c r="H38">
-        <v>0</v>
-      </c>
-      <c r="I38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F38" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>DEN</v>
+      </c>
+      <c r="G38" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>FRA</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2347,20 +2238,16 @@
       <c r="E39">
         <v>4</v>
       </c>
-      <c r="F39" t="s">
-        <v>79</v>
-      </c>
-      <c r="G39" t="s">
-        <v>100</v>
-      </c>
-      <c r="H39">
-        <v>0</v>
-      </c>
-      <c r="I39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F39" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>AUS</v>
+      </c>
+      <c r="G39" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>PER</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2376,20 +2263,16 @@
       <c r="E40">
         <v>3</v>
       </c>
-      <c r="F40" t="s">
-        <v>102</v>
-      </c>
-      <c r="G40" t="s">
-        <v>69</v>
-      </c>
-      <c r="H40">
-        <v>1</v>
-      </c>
-      <c r="I40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F40" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>NGA</v>
+      </c>
+      <c r="G40" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>ARG</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2405,20 +2288,16 @@
       <c r="E41">
         <v>1</v>
       </c>
-      <c r="F41" t="s">
-        <v>101</v>
-      </c>
-      <c r="G41" t="s">
-        <v>76</v>
-      </c>
-      <c r="H41">
-        <v>1</v>
-      </c>
-      <c r="I41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F41" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>ISL</v>
+      </c>
+      <c r="G41" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>CRO</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2434,20 +2313,16 @@
       <c r="E42">
         <v>6</v>
       </c>
-      <c r="F42" t="s">
-        <v>86</v>
-      </c>
-      <c r="G42" t="s">
-        <v>66</v>
-      </c>
-      <c r="H42">
-        <v>0</v>
-      </c>
-      <c r="I42">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F42" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>MEX</v>
+      </c>
+      <c r="G42" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>SWE</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2463,20 +2338,16 @@
       <c r="E43">
         <v>1</v>
       </c>
-      <c r="F43" t="s">
-        <v>82</v>
-      </c>
-      <c r="G43" t="s">
-        <v>85</v>
-      </c>
-      <c r="H43">
-        <v>2</v>
-      </c>
-      <c r="I43">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F43" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>KOR</v>
+      </c>
+      <c r="G43" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>GER</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2492,20 +2363,16 @@
       <c r="E44">
         <v>5</v>
       </c>
-      <c r="F44" t="s">
-        <v>84</v>
-      </c>
-      <c r="G44" t="s">
-        <v>74</v>
-      </c>
-      <c r="H44">
-        <v>2</v>
-      </c>
-      <c r="I44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F44" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>SRB</v>
+      </c>
+      <c r="G44" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>BRA</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2521,20 +2388,16 @@
       <c r="E45">
         <v>2</v>
       </c>
-      <c r="F45" t="s">
-        <v>72</v>
-      </c>
-      <c r="G45" t="s">
-        <v>103</v>
-      </c>
-      <c r="H45">
-        <v>0</v>
-      </c>
-      <c r="I45">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F45" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>SUI</v>
+      </c>
+      <c r="G45" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>CRC</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2550,20 +2413,16 @@
       <c r="E46">
         <v>8</v>
       </c>
-      <c r="F46" t="s">
-        <v>70</v>
-      </c>
-      <c r="G46" t="s">
-        <v>67</v>
-      </c>
-      <c r="H46">
-        <v>0</v>
-      </c>
-      <c r="I46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F46" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>JPN</v>
+      </c>
+      <c r="G46" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>POL</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2579,20 +2438,16 @@
       <c r="E47">
         <v>7</v>
       </c>
-      <c r="F47" t="s">
-        <v>104</v>
-      </c>
-      <c r="G47" t="s">
-        <v>80</v>
-      </c>
-      <c r="H47">
-        <v>1</v>
-      </c>
-      <c r="I47">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F47" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>SEN</v>
+      </c>
+      <c r="G47" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>COL</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2608,20 +2463,16 @@
       <c r="E48">
         <v>1</v>
       </c>
-      <c r="F48" t="s">
-        <v>83</v>
-      </c>
-      <c r="G48" t="s">
-        <v>78</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-      <c r="I48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F48" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>PAN</v>
+      </c>
+      <c r="G48" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>TUN</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2637,20 +2488,16 @@
       <c r="E49">
         <v>9</v>
       </c>
-      <c r="F49" t="s">
-        <v>77</v>
-      </c>
-      <c r="G49" t="s">
-        <v>105</v>
-      </c>
-      <c r="H49">
-        <v>0</v>
-      </c>
-      <c r="I49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F49" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v>ENG</v>
+      </c>
+      <c r="G49" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v>BEL</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2666,20 +2513,16 @@
       <c r="E50">
         <v>4</v>
       </c>
-      <c r="F50" t="s">
-        <v>75</v>
-      </c>
-      <c r="G50" t="s">
-        <v>71</v>
-      </c>
-      <c r="H50">
-        <v>2</v>
-      </c>
-      <c r="I50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F50" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+      <c r="G50" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2695,20 +2538,16 @@
       <c r="E51">
         <v>5</v>
       </c>
-      <c r="F51" t="s">
-        <v>68</v>
-      </c>
-      <c r="G51" t="s">
-        <v>69</v>
-      </c>
-      <c r="H51">
-        <v>4</v>
-      </c>
-      <c r="I51">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F51" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+      <c r="G51" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2724,26 +2563,16 @@
       <c r="E52">
         <v>1</v>
       </c>
-      <c r="F52" t="s">
-        <v>81</v>
-      </c>
-      <c r="G52" t="s">
-        <v>98</v>
-      </c>
-      <c r="H52">
-        <v>1</v>
-      </c>
-      <c r="I52">
-        <v>1</v>
-      </c>
-      <c r="J52">
-        <v>3</v>
-      </c>
-      <c r="K52">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F52" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+      <c r="G52" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2759,26 +2588,16 @@
       <c r="E53">
         <v>1</v>
       </c>
-      <c r="F53" t="s">
-        <v>76</v>
-      </c>
-      <c r="G53" t="s">
-        <v>73</v>
-      </c>
-      <c r="H53">
-        <v>1</v>
-      </c>
-      <c r="I53">
-        <v>1</v>
-      </c>
-      <c r="J53">
-        <v>3</v>
-      </c>
-      <c r="K53">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F53" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+      <c r="G53" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2794,20 +2613,16 @@
       <c r="E54">
         <v>9</v>
       </c>
-      <c r="F54" t="s">
-        <v>66</v>
-      </c>
-      <c r="G54" t="s">
-        <v>72</v>
-      </c>
-      <c r="H54">
-        <v>2</v>
-      </c>
-      <c r="I54">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F54" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+      <c r="G54" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2823,20 +2638,16 @@
       <c r="E55">
         <v>1</v>
       </c>
-      <c r="F55" t="s">
-        <v>67</v>
-      </c>
-      <c r="G55" t="s">
-        <v>83</v>
-      </c>
-      <c r="H55">
-        <v>3</v>
-      </c>
-      <c r="I55">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F55" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+      <c r="G55" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2852,20 +2663,16 @@
       <c r="E56">
         <v>3</v>
       </c>
-      <c r="F56" t="s">
-        <v>103</v>
-      </c>
-      <c r="G56" t="s">
-        <v>82</v>
-      </c>
-      <c r="H56">
-        <v>1</v>
-      </c>
-      <c r="I56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F56" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+      <c r="G56" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2881,26 +2688,16 @@
       <c r="E57">
         <v>6</v>
       </c>
-      <c r="F57" t="s">
-        <v>105</v>
-      </c>
-      <c r="G57" t="s">
-        <v>70</v>
-      </c>
-      <c r="H57">
-        <v>1</v>
-      </c>
-      <c r="I57">
-        <v>1</v>
-      </c>
-      <c r="J57">
-        <v>3</v>
-      </c>
-      <c r="K57">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F57" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+      <c r="G57" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2916,20 +2713,16 @@
       <c r="E58">
         <v>1</v>
       </c>
-      <c r="F58" t="s">
-        <v>75</v>
-      </c>
-      <c r="G58" t="s">
-        <v>68</v>
-      </c>
-      <c r="H58">
-        <v>0</v>
-      </c>
-      <c r="I58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F58" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+      <c r="G58" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2945,20 +2738,16 @@
       <c r="E59">
         <v>5</v>
       </c>
-      <c r="F59" t="s">
-        <v>66</v>
-      </c>
-      <c r="G59" t="s">
-        <v>67</v>
-      </c>
-      <c r="H59">
-        <v>1</v>
-      </c>
-      <c r="I59">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F59" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+      <c r="G59" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2974,26 +2763,16 @@
       <c r="E60">
         <v>4</v>
       </c>
-      <c r="F60" t="s">
-        <v>98</v>
-      </c>
-      <c r="G60" t="s">
-        <v>76</v>
-      </c>
-      <c r="H60">
-        <v>2</v>
-      </c>
-      <c r="I60">
-        <v>2</v>
-      </c>
-      <c r="J60">
-        <v>3</v>
-      </c>
-      <c r="K60">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F60" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+      <c r="G60" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -3009,20 +2788,16 @@
       <c r="E61">
         <v>9</v>
       </c>
-      <c r="F61" t="s">
-        <v>103</v>
-      </c>
-      <c r="G61" t="s">
-        <v>70</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
-      <c r="I61">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F61" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+      <c r="G61" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -3038,20 +2813,16 @@
       <c r="E62">
         <v>3</v>
       </c>
-      <c r="F62" t="s">
-        <v>68</v>
-      </c>
-      <c r="G62" t="s">
-        <v>67</v>
-      </c>
-      <c r="H62">
-        <v>1</v>
-      </c>
-      <c r="I62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F62" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+      <c r="G62" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -3067,20 +2838,16 @@
       <c r="E63">
         <v>1</v>
       </c>
-      <c r="F63" t="s">
-        <v>76</v>
-      </c>
-      <c r="G63" t="s">
-        <v>70</v>
-      </c>
-      <c r="H63">
-        <v>2</v>
-      </c>
-      <c r="I63">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F63" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+      <c r="G63" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -3096,20 +2863,16 @@
       <c r="E64">
         <v>3</v>
       </c>
-      <c r="F64" t="s">
-        <v>67</v>
-      </c>
-      <c r="G64" t="s">
-        <v>70</v>
-      </c>
-      <c r="H64">
-        <v>2</v>
-      </c>
-      <c r="I64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F64" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+      <c r="G64" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -3125,17 +2888,13 @@
       <c r="E65">
         <v>1</v>
       </c>
-      <c r="F65" t="s">
-        <v>68</v>
-      </c>
-      <c r="G65" t="s">
-        <v>76</v>
-      </c>
-      <c r="H65">
-        <v>4</v>
-      </c>
-      <c r="I65">
-        <v>2</v>
+      <c r="F65" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[home-seed]], seeds[seed],0)), "")</f>
+        <v/>
+      </c>
+      <c r="G65" t="str">
+        <f>_xlfn.IFNA(INDEX(seeds[team], MATCH(matches[[#This Row],[away-seed]], seeds[seed],0)), "")</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>